<commit_message>
added ifoCAST full series evaluation
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/2_component_Evaluation_series/first_release_qoq_CONSTR.xlsx
+++ b/0_0_Data/2_Processed_Data/2_component_Evaluation_series/first_release_qoq_CONSTR.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfbe04e23282f0d1/Desktop/ifo/Konjunkturprognose Evaluierung/ifo Forecast Evaluation Workfolder/0_0_Data/2_Processed_Data/2_component_Evaluation_series/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_701D841BCB38910DB6FF31D2F87AE380C805B059" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D4FF57C-1AA8-489F-98FE-3CA2EDA014C0}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -31,11 +25,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,25 +91,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -153,7 +139,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -187,7 +173,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -222,10 +207,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -398,17 +382,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.6328125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -416,15 +397,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>38398</v>
       </c>
       <c r="B2">
-        <v>-3.2263178834294881</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-3.226317883429488</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>38487</v>
       </c>
@@ -432,15 +413,15 @@
         <v>0.5468658301973619</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>38579</v>
       </c>
       <c r="B4">
-        <v>1.8541252974342799</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.85412529743428</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>38671</v>
       </c>
@@ -448,39 +429,39 @@
         <v>2.087368604868217</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>38763</v>
       </c>
       <c r="B6">
-        <v>-4.0089420096517898</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-4.00894200965179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>38852</v>
       </c>
       <c r="B7">
-        <v>7.3312555840536078</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7.331255584053608</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="2">
         <v>38944</v>
       </c>
       <c r="B8">
-        <v>1.9499505069814089</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.949950506981409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="2">
         <v>39036</v>
       </c>
       <c r="B9">
-        <v>1.5051720107002351</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.505172010700235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="2">
         <v>39128</v>
       </c>
@@ -488,23 +469,23 @@
         <v>1.416004207479489</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="2">
         <v>39217</v>
       </c>
       <c r="B11">
-        <v>-3.5180043312949749</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-3.518004331294975</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="2">
         <v>39309</v>
       </c>
       <c r="B12">
-        <v>0.55832629889312102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.558326298893121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="2">
         <v>39401</v>
       </c>
@@ -512,15 +493,15 @@
         <v>-0.5352583396556696</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2">
       <c r="A14" s="2">
         <v>39493</v>
       </c>
       <c r="B14">
-        <v>4.4882265810785213</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4.488226581078521</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="2">
         <v>39583</v>
       </c>
@@ -528,15 +509,15 @@
         <v>-3.397482474306742</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2">
       <c r="A16" s="2">
         <v>39675</v>
       </c>
       <c r="B16">
-        <v>0.27825628515711293</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.2782562851571129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="2">
         <v>39767</v>
       </c>
@@ -544,15 +525,15 @@
         <v>-1.27290341572018</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2">
       <c r="A18" s="2">
         <v>39859</v>
       </c>
       <c r="B18">
-        <v>-2.5899095676207788</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-2.589909567620779</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="2">
         <v>39948</v>
       </c>
@@ -560,7 +541,7 @@
         <v>1.250154354816019</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2">
       <c r="A20" s="2">
         <v>40040</v>
       </c>
@@ -568,7 +549,7 @@
         <v>1.48621908594906</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2">
       <c r="A21" s="2">
         <v>40132</v>
       </c>
@@ -576,31 +557,31 @@
         <v>-0.9550786931962989</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2">
       <c r="A22" s="2">
         <v>40224</v>
       </c>
       <c r="B22">
-        <v>-3.8227690008276198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-3.82276900082762</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="2">
         <v>40313</v>
       </c>
       <c r="B23">
-        <v>6.8533510835182341</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>6.853351083518234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="2">
         <v>40405</v>
       </c>
       <c r="B24">
-        <v>-0.42020080385923109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.4202008038592311</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="2">
         <v>40497</v>
       </c>
@@ -608,23 +589,23 @@
         <v>-2.590749655123886</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2">
       <c r="A26" s="2">
         <v>40589</v>
       </c>
       <c r="B26">
-        <v>6.1905656681758776</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+        <v>6.190565668175878</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="2">
         <v>40678</v>
       </c>
       <c r="B27">
-        <v>-0.37476547290660278</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.3747654729066028</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="2">
         <v>40770</v>
       </c>
@@ -632,15 +613,15 @@
         <v>-0.66979119045169</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2">
       <c r="A29" s="2">
         <v>40862</v>
       </c>
       <c r="B29">
-        <v>1.9007951674699091</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.900795167469909</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="2">
         <v>40954</v>
       </c>
@@ -648,15 +629,15 @@
         <v>-1.346695203931787</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2">
       <c r="A31" s="2">
         <v>41044</v>
       </c>
       <c r="B31">
-        <v>-1.0830978321938569</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-1.083097832193857</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="2">
         <v>41136</v>
       </c>
@@ -664,95 +645,95 @@
         <v>1.527423145498517</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2">
       <c r="A33" s="2">
         <v>41228</v>
       </c>
       <c r="B33">
-        <v>-0.73360692313990228</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.7336069231399023</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="2">
         <v>41320</v>
       </c>
       <c r="B34">
-        <v>-2.0877438668622972</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-2.087743866862297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="2">
         <v>41409</v>
       </c>
       <c r="B35">
-        <v>1.9107946431052909</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.910794643105291</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="2">
         <v>41501</v>
       </c>
       <c r="B36">
-        <v>2.3573262527893921</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2.357326252789392</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="2">
         <v>41593</v>
       </c>
       <c r="B37">
-        <v>0.19527130075813659</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.1952713007581366</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="2">
         <v>41685</v>
       </c>
       <c r="B38">
-        <v>3.6407092583607721</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+        <v>3.640709258360772</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" s="2">
         <v>41774</v>
       </c>
       <c r="B39">
-        <v>-3.8946631766249031</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-3.894663176624903</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="2">
         <v>41866</v>
       </c>
       <c r="B40">
-        <v>-0.34811511303539078</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.3481151130353908</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" s="2">
         <v>41958</v>
       </c>
       <c r="B41">
-        <v>1.3256470822331321</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.325647082233132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" s="2">
         <v>42050</v>
       </c>
       <c r="B42">
-        <v>1.6998893494740059</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.699889349474006</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" s="2">
         <v>42139</v>
       </c>
       <c r="B43">
-        <v>-1.3012407423917409</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-1.301240742391741</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" s="2">
         <v>42231</v>
       </c>
@@ -760,15 +741,15 @@
         <v>-0.3250787905929684</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2">
       <c r="A45" s="2">
         <v>42323</v>
       </c>
       <c r="B45">
-        <v>1.9698906494923849</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.969890649492385</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="2">
         <v>42415</v>
       </c>
@@ -776,79 +757,79 @@
         <v>2.325384209656022</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2">
       <c r="A47" s="2">
         <v>42505</v>
       </c>
       <c r="B47">
-        <v>-1.9072864491145369</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-1.907286449114537</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" s="2">
         <v>42597</v>
       </c>
       <c r="B48">
-        <v>0.27905369259086399</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.279053692590864</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" s="2">
         <v>42689</v>
       </c>
       <c r="B49">
-        <v>0.82378454507872334</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.8237845450787233</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" s="2">
         <v>42781</v>
       </c>
       <c r="B50">
-        <v>2.3001763638837081</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2.300176363883708</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" s="2">
         <v>42870</v>
       </c>
       <c r="B51">
-        <v>0.49490404679413302</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.494904046794133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" s="2">
         <v>42962</v>
       </c>
       <c r="B52">
-        <v>-0.43199430984248011</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.4319943098424801</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" s="2">
         <v>43054</v>
       </c>
       <c r="B53">
-        <v>-0.35732951868206442</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.3573295186820644</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" s="2">
         <v>43146</v>
       </c>
       <c r="B54">
-        <v>2.0720938504834412</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2.072093850483441</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" s="2">
         <v>43235</v>
       </c>
       <c r="B55">
-        <v>0.60915076260161527</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.6091507626016153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" s="2">
         <v>43327</v>
       </c>
@@ -856,15 +837,15 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2">
       <c r="A57" s="2">
         <v>43419</v>
       </c>
       <c r="B57">
-        <v>1.2843230739472771</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.284323073947277</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" s="2">
         <v>43511</v>
       </c>
@@ -872,7 +853,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2">
       <c r="A59" s="2">
         <v>43600</v>
       </c>
@@ -880,71 +861,71 @@
         <v>-1.026414746480526</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2">
       <c r="A60" s="2">
         <v>43692</v>
       </c>
       <c r="B60">
-        <v>1.1729803714303699</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.17298037143037</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" s="2">
         <v>43784</v>
       </c>
       <c r="B61">
-        <v>0.60045005136375096</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.600450051363751</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" s="2">
         <v>43876</v>
       </c>
       <c r="B62">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" s="2">
         <v>43966</v>
       </c>
       <c r="B63">
-        <v>-4.2221334164257476</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-4.222133416425748</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" s="2">
         <v>44058</v>
       </c>
       <c r="B64">
-        <v>-0.39418364537654332</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.3941836453765433</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" s="2">
         <v>44150</v>
       </c>
       <c r="B65">
-        <v>0.88015900873344322</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.8801590087334432</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" s="2">
         <v>44242</v>
       </c>
       <c r="B66">
-        <v>-3.6291698719087719</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-3.629169871908772</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" s="2">
         <v>44331</v>
       </c>
       <c r="B67">
-        <v>0.68794120977229056</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.6879412097722906</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" s="2">
         <v>44423</v>
       </c>
@@ -952,15 +933,15 @@
         <v>1.095591413702294</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2">
       <c r="A69" s="2">
         <v>44515</v>
       </c>
       <c r="B69">
-        <v>0.33758180946708188</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.3375818094670819</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" s="2">
         <v>44607</v>
       </c>
@@ -968,47 +949,47 @@
         <v>2.107773878883052</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2">
       <c r="A71" s="2">
         <v>44696</v>
       </c>
       <c r="B71">
-        <v>-1.5962774036382399</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-1.59627740363824</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" s="2">
         <v>44788</v>
       </c>
       <c r="B72">
-        <v>-0.24299584820830941</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.2429958482083094</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" s="2">
         <v>44880</v>
       </c>
       <c r="B73">
-        <v>-0.50096918047832162</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.5009691804783216</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" s="2">
         <v>44972</v>
       </c>
       <c r="B74">
-        <v>0.63991654879906434</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.6399165487990643</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" s="2">
         <v>45061</v>
       </c>
       <c r="B75">
-        <v>-1.0823925682469731</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-1.082392568246973</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" s="2">
         <v>45153</v>
       </c>
@@ -1016,31 +997,31 @@
         <v>-1.253192088351895</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2">
       <c r="A77" s="2">
         <v>45245</v>
       </c>
       <c r="B77">
-        <v>-1.2252490134152649</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-1.225249013415265</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" s="2">
         <v>45337</v>
       </c>
       <c r="B78">
-        <v>-0.16724919258589921</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.1672491925858992</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79" s="2">
         <v>45427</v>
       </c>
       <c r="B79">
-        <v>-1.3154289065158049</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-1.315428906515805</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" s="2">
         <v>45519</v>
       </c>
@@ -1048,15 +1029,15 @@
         <v>-0.6454450625183199</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2">
       <c r="A81" s="2">
         <v>45611</v>
       </c>
       <c r="B81">
-        <v>-0.36424427368714868</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.3642442736871487</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" s="2">
         <v>45703</v>
       </c>
@@ -1064,15 +1045,15 @@
         <v>-0.2250721972476839</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2">
       <c r="A83" s="2">
         <v>45792</v>
       </c>
       <c r="B83">
-        <v>-4.9946346431113398E-3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.00499463464311134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" s="2">
         <v>45884</v>
       </c>

</xml_diff>

<commit_message>
Fixed naive component forecaster bug - Presentation state 11.02.
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/2_component_Evaluation_series/first_release_qoq_CONSTR.xlsx
+++ b/0_0_Data/2_Processed_Data/2_component_Evaluation_series/first_release_qoq_CONSTR.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfbe04e23282f0d1/Desktop/ifo/Konjunkturprognose Evaluierung/ifo Forecast Evaluation Workfolder/0_0_Data/2_Processed_Data/2_component_Evaluation_series/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_5315841B6048D72196FE31D2F87AE380E885DDA9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA836D00-AE75-4DB5-829A-00FA18A844BB}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -31,11 +25,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,25 +91,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -153,7 +139,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -187,7 +173,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -222,10 +207,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -398,18 +382,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="38.08984375" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -417,15 +397,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>38398</v>
       </c>
       <c r="B2">
-        <v>-3.2263178834294881</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-3.226317883429488</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>38487</v>
       </c>
@@ -433,15 +413,15 @@
         <v>0.5468658301973619</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>38579</v>
       </c>
       <c r="B4">
-        <v>1.8541252974342799</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.85412529743428</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>38671</v>
       </c>
@@ -449,39 +429,39 @@
         <v>2.087368604868217</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>38763</v>
       </c>
       <c r="B6">
-        <v>-4.0089420096517898</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-4.00894200965179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>38852</v>
       </c>
       <c r="B7">
-        <v>7.3312555840536078</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7.331255584053608</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="2">
         <v>38944</v>
       </c>
       <c r="B8">
-        <v>1.9499505069814089</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.949950506981409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="2">
         <v>39036</v>
       </c>
       <c r="B9">
-        <v>1.5051720107002351</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.505172010700235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="2">
         <v>39128</v>
       </c>
@@ -489,23 +469,23 @@
         <v>1.416004207479489</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="2">
         <v>39217</v>
       </c>
       <c r="B11">
-        <v>-3.5180043312949749</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-3.518004331294975</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="2">
         <v>39309</v>
       </c>
       <c r="B12">
-        <v>0.55832629889312102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.558326298893121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="2">
         <v>39401</v>
       </c>
@@ -513,15 +493,15 @@
         <v>-0.5352583396556696</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2">
       <c r="A14" s="2">
         <v>39493</v>
       </c>
       <c r="B14">
-        <v>4.4882265810785213</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4.488226581078521</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="2">
         <v>39583</v>
       </c>
@@ -529,15 +509,15 @@
         <v>-3.397482474306742</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2">
       <c r="A16" s="2">
         <v>39675</v>
       </c>
       <c r="B16">
-        <v>0.27825628515711293</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.2782562851571129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="2">
         <v>39767</v>
       </c>
@@ -545,15 +525,15 @@
         <v>-1.27290341572018</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2">
       <c r="A18" s="2">
         <v>39859</v>
       </c>
       <c r="B18">
-        <v>-2.5899095676207788</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-2.589909567620779</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="2">
         <v>39948</v>
       </c>
@@ -561,7 +541,7 @@
         <v>1.250154354816019</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2">
       <c r="A20" s="2">
         <v>40040</v>
       </c>
@@ -569,7 +549,7 @@
         <v>1.48621908594906</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2">
       <c r="A21" s="2">
         <v>40132</v>
       </c>
@@ -577,31 +557,31 @@
         <v>-0.9550786931962989</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2">
       <c r="A22" s="2">
         <v>40224</v>
       </c>
       <c r="B22">
-        <v>-3.8227690008276198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-3.82276900082762</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="2">
         <v>40313</v>
       </c>
       <c r="B23">
-        <v>6.8533510835182341</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>6.853351083518234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="2">
         <v>40405</v>
       </c>
       <c r="B24">
-        <v>-0.42020080385923109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.4202008038592311</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="2">
         <v>40497</v>
       </c>
@@ -609,23 +589,23 @@
         <v>-2.590749655123886</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2">
       <c r="A26" s="2">
         <v>40589</v>
       </c>
       <c r="B26">
-        <v>6.1905656681758776</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+        <v>6.190565668175878</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="2">
         <v>40678</v>
       </c>
       <c r="B27">
-        <v>-0.37476547290660278</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.3747654729066028</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="2">
         <v>40770</v>
       </c>
@@ -633,15 +613,15 @@
         <v>-0.66979119045169</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2">
       <c r="A29" s="2">
         <v>40862</v>
       </c>
       <c r="B29">
-        <v>1.9007951674699091</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.900795167469909</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="2">
         <v>40954</v>
       </c>
@@ -649,15 +629,15 @@
         <v>-1.346695203931787</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2">
       <c r="A31" s="2">
         <v>41044</v>
       </c>
       <c r="B31">
-        <v>-1.0830978321938569</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-1.083097832193857</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="2">
         <v>41136</v>
       </c>
@@ -665,95 +645,95 @@
         <v>1.527423145498517</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2">
       <c r="A33" s="2">
         <v>41228</v>
       </c>
       <c r="B33">
-        <v>-0.73360692313990228</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.7336069231399023</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="2">
         <v>41320</v>
       </c>
       <c r="B34">
-        <v>-2.0877438668622972</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-2.087743866862297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="2">
         <v>41409</v>
       </c>
       <c r="B35">
-        <v>1.9107946431052909</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.910794643105291</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="2">
         <v>41501</v>
       </c>
       <c r="B36">
-        <v>2.3573262527893921</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2.357326252789392</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="2">
         <v>41593</v>
       </c>
       <c r="B37">
-        <v>0.19527130075813659</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.1952713007581366</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="2">
         <v>41685</v>
       </c>
       <c r="B38">
-        <v>3.6407092583607721</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+        <v>3.640709258360772</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" s="2">
         <v>41774</v>
       </c>
       <c r="B39">
-        <v>-3.8946631766249031</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-3.894663176624903</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="2">
         <v>41866</v>
       </c>
       <c r="B40">
-        <v>-0.34811511303539078</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.3481151130353908</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" s="2">
         <v>41958</v>
       </c>
       <c r="B41">
-        <v>1.3256470822331321</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.325647082233132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" s="2">
         <v>42050</v>
       </c>
       <c r="B42">
-        <v>1.6998893494740059</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.699889349474006</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" s="2">
         <v>42139</v>
       </c>
       <c r="B43">
-        <v>-1.3012407423917409</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-1.301240742391741</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" s="2">
         <v>42231</v>
       </c>
@@ -761,15 +741,15 @@
         <v>-0.3250787905929684</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2">
       <c r="A45" s="2">
         <v>42323</v>
       </c>
       <c r="B45">
-        <v>1.9698906494923849</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.969890649492385</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="2">
         <v>42415</v>
       </c>
@@ -777,79 +757,79 @@
         <v>2.325384209656022</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2">
       <c r="A47" s="2">
         <v>42505</v>
       </c>
       <c r="B47">
-        <v>-1.9072864491145369</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-1.907286449114537</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" s="2">
         <v>42597</v>
       </c>
       <c r="B48">
-        <v>0.27905369259086399</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.279053692590864</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" s="2">
         <v>42689</v>
       </c>
       <c r="B49">
-        <v>0.82378454507872334</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.8237845450787233</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" s="2">
         <v>42781</v>
       </c>
       <c r="B50">
-        <v>2.3001763638837081</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2.300176363883708</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" s="2">
         <v>42870</v>
       </c>
       <c r="B51">
-        <v>0.49490404679413302</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.494904046794133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" s="2">
         <v>42962</v>
       </c>
       <c r="B52">
-        <v>-0.43199430984248011</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.4319943098424801</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" s="2">
         <v>43054</v>
       </c>
       <c r="B53">
-        <v>-0.35732951868206442</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.3573295186820644</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" s="2">
         <v>43146</v>
       </c>
       <c r="B54">
-        <v>2.0720938504834412</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2.072093850483441</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" s="2">
         <v>43235</v>
       </c>
       <c r="B55">
-        <v>0.60915076260161527</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.6091507626016153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" s="2">
         <v>43327</v>
       </c>
@@ -857,15 +837,15 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2">
       <c r="A57" s="2">
         <v>43419</v>
       </c>
       <c r="B57">
-        <v>1.2843230739472771</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.284323073947277</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" s="2">
         <v>43511</v>
       </c>
@@ -873,7 +853,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2">
       <c r="A59" s="2">
         <v>43600</v>
       </c>
@@ -881,39 +861,39 @@
         <v>-1.026414746480526</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2">
       <c r="A60" s="2">
         <v>43692</v>
       </c>
       <c r="B60">
-        <v>1.1729803714303699</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.17298037143037</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" s="2">
         <v>43784</v>
       </c>
       <c r="B61">
-        <v>0.60045005136375096</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.600450051363751</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" s="2">
         <v>43876</v>
       </c>
       <c r="B62">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" s="2">
         <v>43966</v>
       </c>
       <c r="B63">
-        <v>-4.2221334164257476</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-4.222133416425748</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" s="2">
         <v>44058</v>
       </c>
@@ -921,71 +901,71 @@
         <v>-1.967214790670653</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2">
       <c r="A65" s="2">
         <v>44150</v>
       </c>
       <c r="B65">
-        <v>1.8361127474571219</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.836112747457122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" s="2">
         <v>44242</v>
       </c>
       <c r="B66">
-        <v>1.1425072417365669</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.142507241736567</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" s="2">
         <v>44331</v>
       </c>
       <c r="B67">
-        <v>0.27789214681965291</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.2778921468196529</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" s="2">
         <v>44423</v>
       </c>
       <c r="B68">
-        <v>-2.3362116852200638</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-2.336211685220064</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" s="2">
         <v>44515</v>
       </c>
       <c r="B69">
-        <v>3.6429549028966328E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.03642954902896633</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" s="2">
         <v>44607</v>
       </c>
       <c r="B70">
-        <v>4.6230628090513761</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4.623062809051376</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" s="2">
         <v>44696</v>
       </c>
       <c r="B71">
-        <v>-3.3617111509380631</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-3.361711150938063</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" s="2">
         <v>44788</v>
       </c>
       <c r="B72">
-        <v>-1.4329891179920931</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-1.432989117992093</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" s="2">
         <v>44880</v>
       </c>
@@ -993,31 +973,31 @@
         <v>-2.851410521811431</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2">
       <c r="A74" s="2">
         <v>44972</v>
       </c>
       <c r="B74">
-        <v>3.9335573940020789</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+        <v>3.933557394002079</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" s="2">
         <v>45061</v>
       </c>
       <c r="B75">
-        <v>0.23293593589943379</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.2329359358994338</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" s="2">
         <v>45153</v>
       </c>
       <c r="B76">
-        <v>0.43245063494397579</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.4324506349439758</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" s="2">
         <v>45245</v>
       </c>
@@ -1025,7 +1005,7 @@
         <v>-1.721673722292465</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2">
       <c r="A78" s="2">
         <v>45337</v>
       </c>
@@ -1033,15 +1013,15 @@
         <v>2.712662502476618</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2">
       <c r="A79" s="2">
         <v>45427</v>
       </c>
       <c r="B79">
-        <v>-2.0081290002876102</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-2.00812900028761</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" s="2">
         <v>45519</v>
       </c>
@@ -1049,28 +1029,28 @@
         <v>-0.346469331090276</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2">
       <c r="A81" s="2">
         <v>45611</v>
       </c>
       <c r="B81">
-        <v>1.0437122388897959</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.043712238889796</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" s="2">
         <v>45703</v>
       </c>
       <c r="B82">
-        <v>0.52758486034738894</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.5275848603473889</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83" s="2">
         <v>45792</v>
       </c>
       <c r="B83">
-        <v>-2.0734582797890941</v>
+        <v>-2.073458279789094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>